<commit_message>
Fix typo and refactor
Fix typo in explanation method by patient and update style of new chart
</commit_message>
<xml_diff>
--- a/plots/explanation_method_by_patient.xlsx
+++ b/plots/explanation_method_by_patient.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joa24jm\Documents\literature_review\plots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59662FC7-5A03-4744-A7DB-D697D5DA97B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0980A82F-B6F3-4D92-B4CB-055492E26AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{F8619ACE-1305-42D3-B30B-A3DB9A5A58A4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8619ACE-1305-42D3-B30B-A3DB9A5A58A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Understood by patients</t>
   </si>
@@ -60,10 +60,16 @@
     <t>Layer-Wise Relevance Propagation</t>
   </si>
   <si>
-    <t>Saliency Maps</t>
+    <t>Class Activation Mapping or related (i. e., Grad-CAM)</t>
   </si>
   <si>
-    <t>Class Activation Mapping or related</t>
+    <t>Partial Dependence Plots</t>
+  </si>
+  <si>
+    <t>Permutation Importance</t>
+  </si>
+  <si>
+    <t>DeepLift</t>
   </si>
 </sst>
 </file>
@@ -246,11 +252,11 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$A$2:$A$8</c:f>
+              <c:f>Tabelle1!$A$2:$A$10</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>Class Activation Mapping or related</c:v>
+                  <c:v>Class Activation Mapping or related (i. e., Grad-CAM)</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Intrinsic interpretable</c:v>
@@ -265,20 +271,26 @@
                   <c:v>LIME</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>Partial Dependence Plots</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Permutation Importance</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>Layer-Wise Relevance Propagation</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>Saliency Maps</c:v>
+                <c:pt idx="8">
+                  <c:v>DeepLift</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$2:$B$8</c:f>
+              <c:f>Tabelle1!$B$2:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>30</c:v>
                 </c:pt>
@@ -295,10 +307,16 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -389,11 +407,11 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$A$2:$A$8</c:f>
+              <c:f>Tabelle1!$A$2:$A$10</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>Class Activation Mapping or related</c:v>
+                  <c:v>Class Activation Mapping or related (i. e., Grad-CAM)</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Intrinsic interpretable</c:v>
@@ -408,39 +426,51 @@
                   <c:v>LIME</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>Partial Dependence Plots</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Permutation Importance</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>Layer-Wise Relevance Propagation</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>Saliency Maps</c:v>
+                <c:pt idx="8">
+                  <c:v>DeepLift</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$C$2:$C$8</c:f>
+              <c:f>Tabelle1!$C$2:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>84</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
@@ -1584,15 +1614,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03992F78-4E8B-46C5-B417-B41B17009C1C}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="220" zoomScaleNormal="160" zoomScaleSheetLayoutView="220" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScale="131" zoomScaleNormal="160" zoomScaleSheetLayoutView="220" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="64" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1600,18 +1630,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="64" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" ht="99" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2">
         <v>30</v>
       </c>
       <c r="C2" s="2">
-        <v>84</v>
+        <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="48" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1619,10 +1649,10 @@
         <v>21</v>
       </c>
       <c r="C3" s="2">
-        <v>4</v>
+        <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1630,10 +1660,10 @@
         <v>11</v>
       </c>
       <c r="C4" s="2">
-        <v>11</v>
+        <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="80" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" ht="66" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1641,10 +1671,10 @@
         <v>8</v>
       </c>
       <c r="C5" s="2">
-        <v>5</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1652,28 +1682,50 @@
         <v>5</v>
       </c>
       <c r="C6" s="2">
-        <v>13</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="80" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="2">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="32" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2">
         <v>1</v>
       </c>
       <c r="C8" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update figures , perform Chi²
> Update figures with new value counts for saliency maps and attention weights
> perform chi² two compare distribution of code sharing vs data sharing
</commit_message>
<xml_diff>
--- a/plots/explanation_method_by_patient.xlsx
+++ b/plots/explanation_method_by_patient.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joa24jm\Documents\literature_review\plots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0980A82F-B6F3-4D92-B4CB-055492E26AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54441271-7425-4558-B9F0-E4866B2D69C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8619ACE-1305-42D3-B30B-A3DB9A5A58A4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{F8619ACE-1305-42D3-B30B-A3DB9A5A58A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$D$1</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$D$2:$L$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Understood by patients</t>
   </si>
@@ -60,9 +61,6 @@
     <t>Layer-Wise Relevance Propagation</t>
   </si>
   <si>
-    <t>Class Activation Mapping or related (i. e., Grad-CAM)</t>
-  </si>
-  <si>
     <t>Partial Dependence Plots</t>
   </si>
   <si>
@@ -70,6 +68,18 @@
   </si>
   <si>
     <t>DeepLift</t>
+  </si>
+  <si>
+    <t>Saliency Map</t>
+  </si>
+  <si>
+    <t>Attention Weight</t>
+  </si>
+  <si>
+    <t>sum</t>
+  </si>
+  <si>
+    <t>Class Activation Mapping or related</t>
   </si>
 </sst>
 </file>
@@ -215,9 +225,9 @@
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
-                    <a:latin typeface="Bodoni MT" panose="02070603080606020203" pitchFamily="18" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:endParaRPr lang="en-US"/>
@@ -252,71 +262,83 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$A$2:$A$10</c:f>
+              <c:f>Tabelle1!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>Class Activation Mapping or related (i. e., Grad-CAM)</c:v>
+                  <c:v>DeepLift</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Intrinsic interpretable</c:v>
+                  <c:v>Permutation Importance</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>SHAP</c:v>
+                  <c:v>Saliency Map</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Random Forest Feature Importance</c:v>
+                  <c:v>Attention Weight</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>LIME</c:v>
+                  <c:v>Layer-Wise Relevance Propagation</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Partial Dependence Plots</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Permutation Importance</c:v>
+                  <c:v>LIME</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Layer-Wise Relevance Propagation</c:v>
+                  <c:v>Random Forest Feature Importance</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>DeepLift</c:v>
+                  <c:v>Class Activation Mapping or related</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Intrinsic interpretable</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>SHAP</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$2:$B$10</c:f>
+              <c:f>Tabelle1!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -370,9 +392,9 @@
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
-                    <a:latin typeface="Bodoni MT" panose="02070603080606020203" pitchFamily="18" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:endParaRPr lang="en-US"/>
@@ -407,71 +429,83 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$A$2:$A$10</c:f>
+              <c:f>Tabelle1!$A$2:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>Class Activation Mapping or related (i. e., Grad-CAM)</c:v>
+                  <c:v>DeepLift</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Intrinsic interpretable</c:v>
+                  <c:v>Permutation Importance</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>SHAP</c:v>
+                  <c:v>Saliency Map</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Random Forest Feature Importance</c:v>
+                  <c:v>Attention Weight</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>LIME</c:v>
+                  <c:v>Layer-Wise Relevance Propagation</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Partial Dependence Plots</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Permutation Importance</c:v>
+                  <c:v>LIME</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Layer-Wise Relevance Propagation</c:v>
+                  <c:v>Random Forest Feature Importance</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>DeepLift</c:v>
+                  <c:v>Class Activation Mapping or related</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Intrinsic interpretable</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>SHAP</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$C$2:$C$10</c:f>
+              <c:f>Tabelle1!$C$2:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>62</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>73</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>108</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>38</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3</c:v>
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>108</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -531,9 +565,9 @@
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
-                <a:latin typeface="Bodoni MT" panose="02070603080606020203" pitchFamily="18" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -598,9 +632,9 @@
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
-                <a:latin typeface="Bodoni MT" panose="02070603080606020203" pitchFamily="18" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -637,9 +671,9 @@
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:latin typeface="Bodoni MT" panose="02070603080606020203" pitchFamily="18" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+              <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+              <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -674,7 +708,9 @@
           <a:solidFill>
             <a:schemeClr val="tx1"/>
           </a:solidFill>
-          <a:latin typeface="Bodoni MT" panose="02070603080606020203" pitchFamily="18" charset="0"/>
+          <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+          <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+          <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
         </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
@@ -1280,16 +1316,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>275430</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>121183</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>182562</xdr:rowOff>
+      <xdr:rowOff>187409</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>443705</xdr:colOff>
+      <xdr:colOff>564888</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>760412</xdr:rowOff>
+      <xdr:rowOff>765259</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1614,80 +1650,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03992F78-4E8B-46C5-B417-B41B17009C1C}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScale="131" zoomScaleNormal="160" zoomScaleSheetLayoutView="220" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="131" zoomScaleNormal="160" zoomScaleSheetLayoutView="220" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="11.75" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="64" x14ac:dyDescent="0.4">
+      <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" ht="99" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="112" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <f>B2+C2</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="48" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <f>B3+C3</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <f>B4+C4</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="80" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <f>B5+C5</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.4">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <f>B6+C6</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="2">
-        <v>30</v>
-      </c>
-      <c r="C2" s="2">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>21</v>
-      </c>
-      <c r="C3" s="2">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="66" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="B7" s="2">
         <v>2</v>
@@ -1695,41 +1760,91 @@
       <c r="C7" s="2">
         <v>12</v>
       </c>
+      <c r="D7">
+        <f>B7+C7</f>
+        <v>14</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="48" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B8" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C8" s="2">
+        <v>35</v>
+      </c>
+      <c r="D8">
+        <f>B8+C8</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.4">
+      <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B9" s="2">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2">
+        <v>38</v>
+      </c>
+      <c r="D9">
+        <f>B9+C9</f>
+        <v>46</v>
+      </c>
     </row>
-    <row r="9" spans="1:3" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2">
-        <v>1</v>
-      </c>
-      <c r="C9" s="2">
-        <v>8</v>
+    <row r="10" spans="1:4" ht="64" x14ac:dyDescent="0.4">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2">
+        <v>30</v>
+      </c>
+      <c r="C10" s="2">
+        <v>62</v>
+      </c>
+      <c r="D10">
+        <f>B10+C10</f>
+        <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2">
+    <row r="11" spans="1:4" ht="64" x14ac:dyDescent="0.4">
+      <c r="A11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="2">
+        <v>21</v>
+      </c>
+      <c r="C11" s="2">
+        <v>73</v>
+      </c>
+      <c r="D11">
+        <f>B11+C11</f>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.4">
+      <c r="A12" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="B12" s="2">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2">
+        <v>108</v>
+      </c>
+      <c r="D12">
+        <f>B12+C12</f>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D1" xr:uid="{03992F78-4E8B-46C5-B417-B41B17009C1C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D12">
+    <sortCondition ref="D2:D12"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="70" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
add two more figures for ml pipeline description and xai methods
</commit_message>
<xml_diff>
--- a/plots/explanation_method_by_patient.xlsx
+++ b/plots/explanation_method_by_patient.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joa24jm\Documents\literature_review\plots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54441271-7425-4558-B9F0-E4866B2D69C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E482FC-0C68-4DD1-BFC5-045D032AB261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{F8619ACE-1305-42D3-B30B-A3DB9A5A58A4}"/>
+    <workbookView xWindow="-1230" yWindow="-18525" windowWidth="28800" windowHeight="15435" xr2:uid="{F8619ACE-1305-42D3-B30B-A3DB9A5A58A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$D$1</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$D$2:$L$5</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$D$2:$L$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1317,15 +1317,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>121183</xdr:colOff>
+      <xdr:colOff>135837</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>187409</xdr:rowOff>
+      <xdr:rowOff>70177</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>564888</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>765259</xdr:rowOff>
+      <xdr:colOff>579542</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>153865</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1652,18 +1652,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03992F78-4E8B-46C5-B417-B41B17009C1C}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="131" zoomScaleNormal="160" zoomScaleSheetLayoutView="220" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="160" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.75" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
     <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="8.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="64" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1675,7 +1676,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="112" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1686,11 +1687,11 @@
         <v>3</v>
       </c>
       <c r="D2">
-        <f>B2+C2</f>
+        <f t="shared" ref="D2:D12" si="0">B2+C2</f>
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="48" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1701,11 +1702,11 @@
         <v>4</v>
       </c>
       <c r="D3">
-        <f>B3+C3</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" ht="33" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1716,11 +1717,11 @@
         <v>4</v>
       </c>
       <c r="D4">
-        <f>B4+C4</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="80" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" ht="33" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1731,11 +1732,11 @@
         <v>6</v>
       </c>
       <c r="D5">
-        <f>B5+C5</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1746,11 +1747,11 @@
         <v>8</v>
       </c>
       <c r="D6">
-        <f>B6+C6</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1761,11 +1762,11 @@
         <v>12</v>
       </c>
       <c r="D7">
-        <f>B7+C7</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="48" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1776,11 +1777,11 @@
         <v>35</v>
       </c>
       <c r="D8">
-        <f>B8+C8</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -1791,11 +1792,11 @@
         <v>38</v>
       </c>
       <c r="D9">
-        <f>B9+C9</f>
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="64" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -1806,11 +1807,11 @@
         <v>62</v>
       </c>
       <c r="D10">
-        <f>B10+C10</f>
+        <f t="shared" si="0"/>
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="64" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -1821,11 +1822,11 @@
         <v>73</v>
       </c>
       <c r="D11">
-        <f>B11+C11</f>
+        <f t="shared" si="0"/>
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
@@ -1836,7 +1837,7 @@
         <v>108</v>
       </c>
       <c r="D12">
-        <f>B12+C12</f>
+        <f t="shared" si="0"/>
         <v>119</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor fixes on figures legends
</commit_message>
<xml_diff>
--- a/plots/explanation_method_by_patient.xlsx
+++ b/plots/explanation_method_by_patient.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joa24jm\Documents\literature_review\plots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E482FC-0C68-4DD1-BFC5-045D032AB261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A587D475-4356-4FCD-BA98-054259951984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1230" yWindow="-18525" windowWidth="28800" windowHeight="15435" xr2:uid="{F8619ACE-1305-42D3-B30B-A3DB9A5A58A4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8619ACE-1305-42D3-B30B-A3DB9A5A58A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -39,12 +39,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>Understood by patients</t>
-  </si>
-  <si>
-    <t>Not understood by patients</t>
-  </si>
   <si>
     <t>Intrinsic interpretable</t>
   </si>
@@ -80,6 +74,12 @@
   </si>
   <si>
     <t>Class Activation Mapping or related</t>
+  </si>
+  <si>
+    <t>Potentially understanable by patients</t>
+  </si>
+  <si>
+    <t>Not potentially understanable by patients</t>
   </si>
 </sst>
 </file>
@@ -191,7 +191,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Understood by patients</c:v>
+                  <c:v>Potentially understanable by patients</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -358,7 +358,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Not understood by patients</c:v>
+                  <c:v>Not potentially understanable by patients</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1653,7 +1653,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="160" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1664,21 +1664,21 @@
     <col min="12" max="12" width="8.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -1693,7 +1693,7 @@
     </row>
     <row r="3" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -1708,7 +1708,7 @@
     </row>
     <row r="4" spans="1:4" ht="33" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2">
         <v>4</v>
@@ -1723,7 +1723,7 @@
     </row>
     <row r="5" spans="1:4" ht="33" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2">
         <v>2</v>
@@ -1738,7 +1738,7 @@
     </row>
     <row r="6" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
@@ -1753,7 +1753,7 @@
     </row>
     <row r="7" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>2</v>
@@ -1768,7 +1768,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B8" s="2">
         <v>5</v>
@@ -1783,7 +1783,7 @@
     </row>
     <row r="9" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B9" s="2">
         <v>8</v>
@@ -1798,7 +1798,7 @@
     </row>
     <row r="10" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2">
         <v>30</v>
@@ -1813,7 +1813,7 @@
     </row>
     <row r="11" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B11" s="2">
         <v>21</v>
@@ -1828,7 +1828,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B12" s="2">
         <v>11</v>

</xml_diff>